<commit_message>
Review de código requerimiento 0005 y 0006.
</commit_message>
<xml_diff>
--- a/Changarro/ChangarroManager/Plantillas/PlantillaLlena/DatosChangarro.xlsx
+++ b/Changarro/ChangarroManager/Plantillas/PlantillaLlena/DatosChangarro.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="56">
   <si>
     <t xml:space="preserve">Nombre</t>
   </si>
@@ -32,31 +32,154 @@
     <t xml:space="preserve">Existencia</t>
   </si>
   <si>
-    <t xml:space="preserve">MoboBeats</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Audifonos Baratos</t>
+    <t xml:space="preserve">camisa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jdjdffdsh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moda</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zapato</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zapatos moda verano</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hogar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Laptop HP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Laptop Pavilion</t>
   </si>
   <si>
     <t xml:space="preserve">Tecnologia</t>
   </si>
   <si>
-    <t xml:space="preserve">Reproductor MP3 2.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Preproductor de Musica con entrada microSD 2.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Consola 3DS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Consola Portatil Nintendo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tacos al Pastor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bulldog</t>
+    <t xml:space="preserve">Sofa caribu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sofa color tierra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Infantil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Microondas samsung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Microondas ksksk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VideoJuegos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Polo range</t>
+  </si>
+  <si>
+    <t xml:space="preserve">playera  polo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tennis Nike</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tennis Nike Deportivo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Xiaomi lt 9 pro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Xaomi Nueva Generación</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ropero</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ropero de madera</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Refrigerador</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Refrigerador Wirepool</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USB 3.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">USB Tipo C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pantalon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pantalon color caky</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reloj M&amp;M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">jghjgh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Joyas y Relojes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crema para el cabello </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crema para peinar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Belleza</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pants</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pants para atletas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Deportes </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Llanta Good Year</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LLantas para vehiculos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vehiculos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cama</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cama para mascotas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Macota</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Intense</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Perfume para caballero</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Perfumeria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tocador</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tocador para cuarto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Muebleria</t>
   </si>
 </sst>
 </file>
@@ -106,8 +229,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="52.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="10.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="24.33203125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="8.5" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="13.1640625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="9.5" bestFit="1" customWidth="1" collapsed="1"/>
@@ -142,7 +265,7 @@
         <v>7</v>
       </c>
       <c r="C2">
-        <v>30</v>
+        <v>6800</v>
       </c>
       <c r="D2" t="s">
         <v>8</v>
@@ -162,56 +285,356 @@
         <v>10</v>
       </c>
       <c r="C3">
-        <v>50</v>
+        <v>7600</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E3" t="b">
         <v>1</v>
       </c>
       <c r="F3">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C4">
-        <v>1000</v>
+        <v>14999</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="E4" t="b">
         <v>1</v>
       </c>
       <c r="F4">
-        <v>10</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5">
+        <v>22000</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6">
+        <v>12999</v>
+      </c>
+      <c r="D6" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" t="b">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7">
+        <v>450</v>
+      </c>
+      <c r="D7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" t="b">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8">
+        <v>1600</v>
+      </c>
+      <c r="D8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" t="b">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9">
+        <v>8599</v>
+      </c>
+      <c r="D9" t="s">
         <v>14</v>
       </c>
-      <c r="C5">
+      <c r="E9" t="b">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C10">
+        <v>3499</v>
+      </c>
+      <c r="D10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" t="b">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11">
+        <v>9999</v>
+      </c>
+      <c r="D11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E11" t="b">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12">
+        <v>200</v>
+      </c>
+      <c r="D12" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" t="b">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B13" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13">
+        <v>600</v>
+      </c>
+      <c r="D13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" t="b">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>35</v>
+      </c>
+      <c r="B14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14">
+        <v>670</v>
+      </c>
+      <c r="D14" t="s">
+        <v>37</v>
+      </c>
+      <c r="E14" t="b">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" t="s">
+        <v>39</v>
+      </c>
+      <c r="C15">
+        <v>340</v>
+      </c>
+      <c r="D15" t="s">
+        <v>40</v>
+      </c>
+      <c r="E15" t="b">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16">
+        <v>780</v>
+      </c>
+      <c r="D16" t="s">
+        <v>43</v>
+      </c>
+      <c r="E16" t="b">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" t="s">
+        <v>45</v>
+      </c>
+      <c r="C17">
+        <v>3000</v>
+      </c>
+      <c r="D17" t="s">
+        <v>46</v>
+      </c>
+      <c r="E17" t="b">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18">
+        <v>230</v>
+      </c>
+      <c r="D18" t="s">
+        <v>49</v>
+      </c>
+      <c r="E18" t="b">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19">
+        <v>4579</v>
+      </c>
+      <c r="D19" t="s">
+        <v>52</v>
+      </c>
+      <c r="E19" t="b">
+        <v>1</v>
+      </c>
+      <c r="F19">
         <v>5</v>
       </c>
-      <c r="D5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" t="b">
-        <v>1</v>
-      </c>
-      <c r="F5">
-        <v>1000</v>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>53</v>
+      </c>
+      <c r="B20" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20">
+        <v>36000</v>
+      </c>
+      <c r="D20" t="s">
+        <v>55</v>
+      </c>
+      <c r="E20" t="b">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modifique la vista de compra y la de productos.
</commit_message>
<xml_diff>
--- a/Changarro/ChangarroManager/Plantillas/PlantillaLlena/DatosChangarro.xlsx
+++ b/Changarro/ChangarroManager/Plantillas/PlantillaLlena/DatosChangarro.xlsx
@@ -174,7 +174,7 @@
         <v>1</v>
       </c>
       <c r="F3">
-        <v>35</v>
+        <v>150</v>
       </c>
     </row>
     <row r="4">
@@ -214,7 +214,7 @@
         <v>1</v>
       </c>
       <c r="F5">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>